<commit_message>
Restructured the code files
</commit_message>
<xml_diff>
--- a/Results/Control_GenComparison_SignificanceTests.xlsx
+++ b/Results/Control_GenComparison_SignificanceTests.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,14 +478,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>246.5080377406668</v>
+        <v>103.9250343758279</v>
       </c>
       <c r="E2" t="n">
-        <v>2.961145395259575e-54</v>
+        <v>5.450084891987035e-43</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -504,14 +504,14 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>646.0073268442724</v>
+        <v>492.2975528874661</v>
       </c>
       <c r="E3" t="n">
-        <v>5.263702571353601e-141</v>
+        <v>4.982197960906943e-165</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -530,14 +530,14 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1008.982590629773</v>
+        <v>2488.279675972683</v>
       </c>
       <c r="E4" t="n">
-        <v>7.983885069507033e-220</v>
+        <v>0</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -556,14 +556,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>21.92136763872862</v>
+        <v>36.80602324941301</v>
       </c>
       <c r="E5" t="n">
-        <v>1.737142714911184e-05</v>
+        <v>2.488443800449051e-16</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -582,14 +582,14 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>963.3572968805995</v>
+        <v>1865.500228308488</v>
       </c>
       <c r="E6" t="n">
-        <v>6.450909240872693e-210</v>
+        <v>0</v>
       </c>
       <c r="F6" t="b">
         <v>1</v>
@@ -608,14 +608,14 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>637.0271315612107</v>
+        <v>340.6284512531364</v>
       </c>
       <c r="E7" t="n">
-        <v>4.691545905702996e-139</v>
+        <v>1.199104472394488e-122</v>
       </c>
       <c r="F7" t="b">
         <v>1</v>
@@ -634,14 +634,14 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>156.5982558062737</v>
+        <v>93.14539548606869</v>
       </c>
       <c r="E8" t="n">
-        <v>9.88828132689099e-35</v>
+        <v>7.471291394604005e-39</v>
       </c>
       <c r="F8" t="b">
         <v>1</v>
@@ -660,14 +660,14 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>76.97069517916204</v>
+        <v>17.23422415869616</v>
       </c>
       <c r="E9" t="n">
-        <v>1.932083571486454e-17</v>
+        <v>3.982348758822768e-08</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -686,14 +686,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>50.82343839211201</v>
+        <v>4.10521155535292</v>
       </c>
       <c r="E10" t="n">
-        <v>9.200905654095116e-12</v>
+        <v>0.01667249606816113</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -712,14 +712,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>10.11640746995032</v>
+        <v>24.28869629620745</v>
       </c>
       <c r="E11" t="n">
-        <v>0.006356968062847287</v>
+        <v>4.159931931841053e-11</v>
       </c>
       <c r="F11" t="b">
         <v>1</v>
@@ -738,14 +738,14 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>458.7354542924413</v>
+        <v>259.0150279682046</v>
       </c>
       <c r="E12" t="n">
-        <v>2.437035040755961e-100</v>
+        <v>2.504918173677693e-97</v>
       </c>
       <c r="F12" t="b">
         <v>1</v>
@@ -764,14 +764,14 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Kruskal Wallis H test</t>
+          <t>One-way F test</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>492.2182209379289</v>
+        <v>292.7912155427557</v>
       </c>
       <c r="E13" t="n">
-        <v>1.306686418734429e-107</v>
+        <v>4.783773674273814e-108</v>
       </c>
       <c r="F13" t="b">
         <v>1</v>
@@ -790,14 +790,14 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>26720.5</v>
+        <v>-3.20007098844747</v>
       </c>
       <c r="E14" t="n">
-        <v>0.004962198183433836</v>
+        <v>0.001461579957827798</v>
       </c>
       <c r="F14" t="b">
         <v>1</v>
@@ -816,14 +816,14 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>26571</v>
+        <v>-4.62777566626418</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0004746132808820661</v>
+        <v>4.72011467708349e-06</v>
       </c>
       <c r="F15" t="b">
         <v>1</v>
@@ -842,14 +842,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>38625</v>
+        <v>5.292175244158653</v>
       </c>
       <c r="E16" t="n">
-        <v>4.797921808714724e-06</v>
+        <v>1.815062139272068e-07</v>
       </c>
       <c r="F16" t="b">
         <v>1</v>
@@ -894,14 +894,14 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>25988</v>
+        <v>-4.366461921739277</v>
       </c>
       <c r="E18" t="n">
-        <v>0.001121306144358755</v>
+        <v>1.536775195372723e-05</v>
       </c>
       <c r="F18" t="b">
         <v>1</v>
@@ -946,14 +946,14 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>35777.5</v>
+        <v>2.897497209476683</v>
       </c>
       <c r="E20" t="n">
-        <v>0.005071138681623663</v>
+        <v>0.003927216464984266</v>
       </c>
       <c r="F20" t="b">
         <v>1</v>
@@ -998,14 +998,14 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>37892</v>
+        <v>3.557182660562407</v>
       </c>
       <c r="E22" t="n">
-        <v>3.914878028815284e-05</v>
+        <v>0.000410682646011469</v>
       </c>
       <c r="F22" t="b">
         <v>1</v>
@@ -1024,14 +1024,14 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>31060</v>
+        <v>-0.867142270016976</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9056732435514132</v>
+        <v>0.3862816838368289</v>
       </c>
       <c r="F23" t="b">
         <v>0</v>
@@ -1050,14 +1050,14 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>10314</v>
+        <v>-15.17561716272611</v>
       </c>
       <c r="E24" t="n">
-        <v>1.863379947676896e-38</v>
+        <v>4.968122309413295e-43</v>
       </c>
       <c r="F24" t="b">
         <v>1</v>
@@ -1076,14 +1076,14 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>52685</v>
+        <v>15.41329739875774</v>
       </c>
       <c r="E25" t="n">
-        <v>3.232232955229114e-40</v>
+        <v>4.144656743666704e-44</v>
       </c>
       <c r="F25" t="b">
         <v>1</v>
@@ -1102,14 +1102,14 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>36123</v>
+        <v>3.63490470761788</v>
       </c>
       <c r="E26" t="n">
-        <v>0.002551523844637625</v>
+        <v>0.0003069922751638511</v>
       </c>
       <c r="F26" t="b">
         <v>1</v>
@@ -1128,14 +1128,14 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>25602</v>
+        <v>-3.879525504622102</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0004706952286676546</v>
+        <v>0.0001187192107984613</v>
       </c>
       <c r="F27" t="b">
         <v>1</v>
@@ -1154,14 +1154,14 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>36407</v>
+        <v>3.703629135984921</v>
       </c>
       <c r="E28" t="n">
-        <v>0.001324248358657921</v>
+        <v>0.000236309863528453</v>
       </c>
       <c r="F28" t="b">
         <v>1</v>
@@ -1180,14 +1180,14 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>33565</v>
+        <v>0.5409203513035115</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1519099220631196</v>
+        <v>0.5888043460659246</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -1206,14 +1206,14 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>25491.5</v>
+        <v>-3.226509327587789</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0003644835402137449</v>
+        <v>0.001335558424313903</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
@@ -1232,14 +1232,14 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>36421.5</v>
+        <v>3.789572000834149</v>
       </c>
       <c r="E31" t="n">
-        <v>0.001368680884196794</v>
+        <v>0.0001693798411145114</v>
       </c>
       <c r="F31" t="b">
         <v>1</v>
@@ -1258,14 +1258,14 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>30806.5</v>
+        <v>-0.2054382678130561</v>
       </c>
       <c r="E32" t="n">
-        <v>0.783897677985003</v>
+        <v>0.8373136719515815</v>
       </c>
       <c r="F32" t="b">
         <v>0</v>
@@ -1284,14 +1284,14 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>31533</v>
+        <v>0.4464872046650555</v>
       </c>
       <c r="E33" t="n">
-        <v>0.8611700668362117</v>
+        <v>0.6554394366694096</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -1310,14 +1310,14 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>31294.5</v>
+        <v>0.6760445824019018</v>
       </c>
       <c r="E34" t="n">
-        <v>0.9782563092214459</v>
+        <v>0.4993261673274386</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -1336,14 +1336,14 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>34173</v>
+        <v>1.2416706355686</v>
       </c>
       <c r="E35" t="n">
-        <v>0.06498746528289231</v>
+        <v>0.2149425882217344</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -1362,17 +1362,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>34024.5</v>
+        <v>1.967883838387863</v>
       </c>
       <c r="E36" t="n">
-        <v>0.08579121679377574</v>
+        <v>0.04963582312876014</v>
       </c>
       <c r="F36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37">
@@ -1388,14 +1388,14 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>28976.5</v>
+        <v>-1.210112196764809</v>
       </c>
       <c r="E37" t="n">
-        <v>0.1592683586279064</v>
+        <v>0.22680991195355</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -1414,14 +1414,14 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>4161.5</v>
+        <v>-26.70903432385005</v>
       </c>
       <c r="E38" t="n">
-        <v>3.799084875195397e-74</v>
+        <v>3.478876148824275e-98</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
@@ -1440,14 +1440,14 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>56349</v>
+        <v>22.40540323826895</v>
       </c>
       <c r="E39" t="n">
-        <v>1.605082722621865e-65</v>
+        <v>2.050111511544678e-77</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -1466,14 +1466,14 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>52750</v>
+        <v>18.07577900150219</v>
       </c>
       <c r="E40" t="n">
-        <v>1.228972019498562e-55</v>
+        <v>1.587913225899474e-56</v>
       </c>
       <c r="F40" t="b">
         <v>1</v>
@@ -1492,14 +1492,14 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>6967</v>
+        <v>-20.3533957131679</v>
       </c>
       <c r="E41" t="n">
-        <v>1.948602220426269e-51</v>
+        <v>1.836427519341772e-67</v>
       </c>
       <c r="F41" t="b">
         <v>1</v>
@@ -1518,14 +1518,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>56930</v>
+        <v>23.35243727784407</v>
       </c>
       <c r="E42" t="n">
-        <v>2.631128222983391e-57</v>
+        <v>5.19572498798019e-82</v>
       </c>
       <c r="F42" t="b">
         <v>1</v>
@@ -1544,14 +1544,14 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>6002</v>
+        <v>-24.28682441786492</v>
       </c>
       <c r="E43" t="n">
-        <v>4.54606700553853e-55</v>
+        <v>1.547847087079104e-86</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
@@ -1570,14 +1570,14 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>27197.5</v>
+        <v>-2.016040750719476</v>
       </c>
       <c r="E44" t="n">
-        <v>0.01212658638000735</v>
+        <v>0.04433218659223444</v>
       </c>
       <c r="F44" t="b">
         <v>1</v>
@@ -1596,14 +1596,14 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>39276</v>
+        <v>2.659495576454042</v>
       </c>
       <c r="E45" t="n">
-        <v>6.755221607885951e-07</v>
+        <v>0.008077905587840311</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
@@ -1622,14 +1622,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>33983.5</v>
+        <v>-0.8638296036201208</v>
       </c>
       <c r="E46" t="n">
-        <v>0.09060432573605678</v>
+        <v>0.3880973580777607</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
@@ -1648,17 +1648,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>25154.5</v>
+        <v>-1.921300344464408</v>
       </c>
       <c r="E47" t="n">
-        <v>0.0001494927491429301</v>
+        <v>0.05526432420963388</v>
       </c>
       <c r="F47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1674,14 +1674,14 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>8196</v>
+        <v>-13.99724859110737</v>
       </c>
       <c r="E48" t="n">
-        <v>3.105342466098088e-46</v>
+        <v>8.894914808069599e-38</v>
       </c>
       <c r="F48" t="b">
         <v>1</v>
@@ -1700,16 +1700,328 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Mann Whitney U test</t>
+          <t>T-Test</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>53980.5</v>
+        <v>13.79218912698009</v>
       </c>
       <c r="E49" t="n">
-        <v>5.471031451978363e-45</v>
+        <v>7.004891698637221e-37</v>
       </c>
       <c r="F49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>ratio_paras</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>337.1931345863907</v>
+      </c>
+      <c r="E50" t="n">
+        <v>5.072061204772169e-242</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>ratio_list_items</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>503.0133287261479</v>
+      </c>
+      <c r="E51" t="n">
+        <v>4.474863225088838e-317</v>
+      </c>
+      <c r="F51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>ratio_headings</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1434.350177387523</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>avg_para_len</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>121.9227978430191</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2.327858259410091e-108</v>
+      </c>
+      <c r="F53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>num_sentences</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>854.5093066193562</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>avg_len</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>600.8964257179297</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>flesch</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>40.10816492550137</v>
+      </c>
+      <c r="E56" t="n">
+        <v>8.742930203466194e-39</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>cli</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>11.30245280737467</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1.017809412477035e-10</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>avg_concrete</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>2.65397987484021</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.02136283399874483</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>concrete_ratio</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>11.670469474077</v>
+      </c>
+      <c r="E59" t="n">
+        <v>4.38810462932117e-11</v>
+      </c>
+      <c r="F59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>abstract_ratio</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>221.1192272393743</v>
+      </c>
+      <c r="E60" t="n">
+        <v>8.646651848982935e-177</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>IAS</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>undefined_ratio</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>One-way F test</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>228.4717117168348</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2.473556392891394e-181</v>
+      </c>
+      <c r="F61" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>